<commit_message>
results updated for without stopword
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bc1dfb5cace04768/Documents/SIT/INF2008/INF2008_YelpZip/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="8_{C1BDD932-E9D8-4EE2-A24B-9B79FCB516DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58F0A227-4D20-4202-B4BA-DA352F680E40}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="8_{C1BDD932-E9D8-4EE2-A24B-9B79FCB516DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC4A4E37-81C3-48D7-80EB-D6BFB2E8BC74}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{523C0EBC-3B2C-48ED-B2D8-8FB42A6877EA}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{523C0EBC-3B2C-48ED-B2D8-8FB42A6877EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="24">
   <si>
     <t>Accuracy</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>Before Feature Engineering (MinMaxScaler)</t>
+  </si>
+  <si>
+    <t>Random Forest</t>
   </si>
 </sst>
 </file>
@@ -526,11 +529,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B68A547D-3863-426E-8B65-5D018732EA23}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,6 +983,35 @@
       </c>
       <c r="I18" s="10">
         <v>0.72499999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="8">
+        <v>0.8669</v>
+      </c>
+      <c r="F19" s="9">
+        <v>0.44</v>
+      </c>
+      <c r="G19" s="9">
+        <v>0.03</v>
+      </c>
+      <c r="H19" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="I19" s="10">
+        <v>0.6583</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated with models trained(svd)
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanwei23/Documents/GitHub/INF2008_YelpZip/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B363331A-DF1F-8746-9FEA-A35C4954A910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F8BF9F-B2D4-9843-9689-DF9113585141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="520" windowWidth="17820" windowHeight="18800" xr2:uid="{523C0EBC-3B2C-48ED-B2D8-8FB42A6877EA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="17820" windowHeight="18800" xr2:uid="{523C0EBC-3B2C-48ED-B2D8-8FB42A6877EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="31">
   <si>
     <t>Accuracy</t>
   </si>
@@ -117,6 +117,18 @@
   </si>
   <si>
     <t>SVM (Linear)</t>
+  </si>
+  <si>
+    <t>SGDClassifier (log_loss)</t>
+  </si>
+  <si>
+    <t>SVD</t>
+  </si>
+  <si>
+    <t>SVD + MinMaxScaler</t>
+  </si>
+  <si>
+    <t>SVD + MinMaxScaler + Undersampling</t>
   </si>
 </sst>
 </file>
@@ -148,7 +160,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -171,11 +183,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -204,13 +227,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -547,11 +569,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B68A547D-3863-426E-8B65-5D018732EA23}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J23" sqref="J23"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1037,7 +1059,7 @@
       <c r="B20" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="3" t="s">
@@ -1046,16 +1068,16 @@
       <c r="E20" s="8">
         <v>0.67720000000000002</v>
       </c>
-      <c r="F20" s="13">
+      <c r="F20" s="9">
         <v>0.24</v>
       </c>
-      <c r="G20" s="13">
+      <c r="G20" s="9">
         <v>0.68</v>
       </c>
-      <c r="H20" s="13">
+      <c r="H20" s="9">
         <v>0.36</v>
       </c>
-      <c r="I20" s="14">
+      <c r="I20" s="10">
         <v>0.74080000000000001</v>
       </c>
     </row>
@@ -1064,7 +1086,7 @@
       <c r="B21" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D21" s="3" t="s">
@@ -1082,7 +1104,7 @@
       <c r="H21" s="9">
         <v>0.34</v>
       </c>
-      <c r="I21" s="14">
+      <c r="I21" s="10">
         <v>0.71630000000000005</v>
       </c>
     </row>
@@ -1091,10 +1113,10 @@
       <c r="B22" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="3" t="s">
         <v>26</v>
       </c>
       <c r="E22" s="4">
@@ -1116,10 +1138,10 @@
       <c r="B23" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="3" t="s">
         <v>26</v>
       </c>
       <c r="E23" s="4">
@@ -1135,6 +1157,84 @@
         <v>0.34</v>
       </c>
       <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="B24" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="13">
+        <v>0.85760000000000003</v>
+      </c>
+      <c r="F24" s="14">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G24" s="14">
+        <v>0.06</v>
+      </c>
+      <c r="H24" s="14">
+        <v>0.09</v>
+      </c>
+      <c r="I24" s="15">
+        <v>0.61909999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="B25" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" s="13">
+        <v>0.8679</v>
+      </c>
+      <c r="F25" s="14">
+        <v>0.52</v>
+      </c>
+      <c r="G25" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="H25" s="14">
+        <v>0.02</v>
+      </c>
+      <c r="I25" s="15">
+        <v>0.73219999999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="B26" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" s="13">
+        <v>0.13220000000000001</v>
+      </c>
+      <c r="F26" s="14">
+        <v>0.13</v>
+      </c>
+      <c r="G26" s="14">
+        <v>1</v>
+      </c>
+      <c r="H26" s="14">
+        <v>0.23</v>
+      </c>
+      <c r="I26" s="15">
+        <v>0.46</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>